<commit_message>
Solicitud rec 340 ma_11_06_co
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion06/SolicitudGrafica MA_11_06_REC340_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion06/SolicitudGrafica MA_11_06_REC340_CO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joan/Dropbox/Aula planeta/Entregas/Entrega 25 (cuenta para agosto) X/REC340 (M101AP)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,8 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="199">
   <si>
     <t>Fecha:</t>
   </si>
@@ -641,7 +638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -807,6 +804,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1355,7 +1358,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1677,6 +1680,7 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1783,7 +1787,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1805,13 +1809,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1041400</xdr:colOff>
+          <xdr:colOff>1038225</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -1860,13 +1864,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1054100</xdr:colOff>
+          <xdr:colOff>1057275</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>863600</xdr:colOff>
+          <xdr:colOff>866775</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -1915,7 +1919,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1972,13 +1976,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1016000</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2025,15 +2029,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1016000</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2082,13 +2086,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2137,13 +2141,13 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2510,34 +2514,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.83203125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="10.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="2"/>
+    <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2556,7 +2560,7 @@
         <v>Ubicación de la imagen en el recurso M101</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
@@ -2587,7 +2591,7 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2616,7 +2620,7 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2648,7 +2652,7 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2679,7 +2683,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2703,7 +2707,7 @@
         <v>M8A</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
@@ -2732,7 +2736,7 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2759,7 +2763,7 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="38.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -2799,7 +2803,7 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -2844,7 +2848,7 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2889,7 +2893,7 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
@@ -2926,15 +2930,15 @@
       <c r="J12" s="78" t="s">
         <v>192</v>
       </c>
-      <c r="K12" s="64" t="s">
-        <v>198</v>
+      <c r="K12" s="110">
+        <v>422100022</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
@@ -2971,15 +2975,15 @@
       <c r="J13" s="78" t="s">
         <v>193</v>
       </c>
-      <c r="K13" s="64" t="s">
-        <v>198</v>
+      <c r="K13" s="110">
+        <v>163407914</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3016,15 +3020,15 @@
       <c r="J14" s="78" t="s">
         <v>194</v>
       </c>
-      <c r="K14" s="64" t="s">
-        <v>198</v>
+      <c r="K14" s="110">
+        <v>68915437</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
@@ -3069,7 +3073,7 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
@@ -3114,7 +3118,7 @@
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
@@ -3159,7 +3163,7 @@
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3194,7 +3198,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
@@ -3229,7 +3233,7 @@
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3264,7 +3268,7 @@
         <v>F10B</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3299,7 +3303,7 @@
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3334,7 +3338,7 @@
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3369,7 +3373,7 @@
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3404,7 +3408,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3435,7 +3439,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3466,7 +3470,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3498,7 +3502,7 @@
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3529,7 +3533,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3560,7 +3564,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3591,7 +3595,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3622,7 +3626,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3653,7 +3657,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3684,7 +3688,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3716,7 +3720,7 @@
       <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3748,7 +3752,7 @@
       <c r="K35" s="65"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3780,7 +3784,7 @@
       <c r="K36" s="65"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3811,7 +3815,7 @@
       <c r="J37" s="70"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3842,7 +3846,7 @@
       <c r="J38" s="71"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3873,7 +3877,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3904,7 +3908,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3935,7 +3939,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3966,7 +3970,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3997,7 +4001,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4028,7 +4032,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4059,7 +4063,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4090,7 +4094,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4121,7 +4125,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4152,7 +4156,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4183,7 +4187,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4214,7 +4218,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4245,7 +4249,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4276,7 +4280,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4307,7 +4311,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4338,7 +4342,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4369,7 +4373,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4400,7 +4404,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4431,7 +4435,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4462,7 +4466,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4493,7 +4497,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4524,7 +4528,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4555,7 +4559,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4586,7 +4590,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4617,7 +4621,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4648,7 +4652,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4679,7 +4683,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4710,7 +4714,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4741,7 +4745,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4772,7 +4776,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4803,7 +4807,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4834,7 +4838,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4865,7 +4869,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4896,7 +4900,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4927,7 +4931,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4958,7 +4962,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4989,7 +4993,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5020,7 +5024,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5051,7 +5055,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5082,7 +5086,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5113,7 +5117,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5144,7 +5148,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5175,7 +5179,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5206,7 +5210,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5237,7 +5241,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5268,7 +5272,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5299,7 +5303,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5330,7 +5334,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5361,7 +5365,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5392,7 +5396,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5423,7 +5427,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5454,7 +5458,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5485,7 +5489,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5516,7 +5520,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5547,7 +5551,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5578,7 +5582,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5609,7 +5613,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5640,7 +5644,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5671,7 +5675,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5702,7 +5706,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5733,7 +5737,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5764,7 +5768,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5795,7 +5799,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5826,7 +5830,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5857,7 +5861,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5888,7 +5892,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5919,7 +5923,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5950,7 +5954,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5981,7 +5985,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6059,25 +6063,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.1640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="22"/>
-    <col min="3" max="3" width="13.83203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="22" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="22"/>
+    <col min="1" max="1" width="72.125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="22"/>
+    <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="22" customWidth="1"/>
+    <col min="5" max="7" width="10.875" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="22"/>
+    <col min="12" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
@@ -6087,7 +6091,7 @@
       <c r="E1" s="95"/>
       <c r="F1" s="96"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
@@ -6099,7 +6103,7 @@
       <c r="E2" s="99"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
@@ -6123,7 +6127,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6151,7 +6155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6178,7 +6182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6200,7 +6204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6227,7 +6231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6246,7 +6250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6265,7 +6269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6284,7 +6288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6295,7 +6299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6306,7 +6310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="94" t="s">
         <v>41</v>
       </c>
@@ -6325,7 +6329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6342,7 +6346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -6360,7 +6364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6384,7 +6388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6405,7 +6409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6426,7 +6430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6445,7 +6449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6467,7 +6471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6484,122 +6488,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6633,19 +6637,18 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1016000</xdr:colOff>
+                    <xdr:colOff>1019175</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6654,21 +6657,20 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1016000</xdr:colOff>
+                    <xdr:colOff>1019175</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6679,19 +6681,18 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6702,19 +6703,18 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6723,13 +6723,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1041400</xdr:colOff>
+                    <xdr:colOff>1038225</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -6737,7 +6737,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6746,13 +6745,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1054100</xdr:colOff>
+                    <xdr:colOff>1057275</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>863600</xdr:colOff>
+                    <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -6760,7 +6759,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6769,7 +6767,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -6783,11 +6781,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
 </worksheet>
 </file>
@@ -6801,22 +6797,22 @@
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.125" style="22" customWidth="1"/>
     <col min="3" max="3" width="17" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.125" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="22"/>
+    <col min="11" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="109" t="s">
         <v>56</v>
       </c>
@@ -6843,7 +6839,7 @@
       </c>
       <c r="I1" s="108"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="109"/>
       <c r="B2" s="109"/>
       <c r="C2" s="109"/>
@@ -6858,7 +6854,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -6883,7 +6879,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -6912,7 +6908,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -6941,7 +6937,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -6970,7 +6966,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -6995,7 +6991,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -7024,7 +7020,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -7053,7 +7049,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -7082,7 +7078,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -7107,7 +7103,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -7136,7 +7132,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7165,7 +7161,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7188,7 +7184,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>96</v>
       </c>
@@ -7214,7 +7210,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7242,7 +7238,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7270,7 +7266,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7296,7 +7292,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7320,7 +7316,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7344,7 +7340,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7368,7 +7364,7 @@
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7392,7 +7388,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7421,7 +7417,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7444,7 +7440,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
-    <row r="25" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7468,7 +7464,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7497,7 +7493,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7521,7 +7517,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7545,7 +7541,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7574,7 +7570,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7597,7 +7593,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7614,7 +7610,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7629,7 +7625,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7650,7 +7646,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7667,7 +7663,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7696,7 +7692,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7725,7 +7721,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7748,7 +7744,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7771,13 +7767,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7791,7 +7787,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -7805,7 +7801,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -7819,7 +7815,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7833,7 +7829,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -7847,7 +7843,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>

</xml_diff>